<commit_message>
Update project code and packages
</commit_message>
<xml_diff>
--- a/Blog-Skeleton/UI.tests/DataDrivenTests/RegistrationUser.xlsx
+++ b/Blog-Skeleton/UI.tests/DataDrivenTests/RegistrationUser.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\QA-courseWork\QAProjectRepo\Blog-Skeleton\UI.tests\DataDrivenTests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="16830" windowHeight="6465"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Key</t>
   </si>
@@ -59,12 +64,33 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>user@abv.bg</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>password1</t>
+  </si>
+  <si>
+    <t>RegisterMIsmatchPassword</t>
+  </si>
+  <si>
+    <t>RegisterWithoutFullName</t>
+  </si>
+  <si>
+    <t>RegisterWithoutPassword</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
@@ -155,6 +181,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -202,7 +231,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -235,9 +264,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -270,6 +316,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -446,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -483,7 +546,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -503,7 +566,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -523,7 +586,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -539,6 +602,57 @@
       </c>
       <c r="F4" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>